<commit_message>
Preliminary mapping of several resources
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-HealthcareAgent.xlsx
+++ b/output/StructureDefinition-PADI-HealthcareAgent.xlsx
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>47</v>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>41</v>
@@ -2425,10 +2425,10 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>39</v>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>41</v>

</xml_diff>